<commit_message>
Added Meeting Minutes and Datasets
</commit_message>
<xml_diff>
--- a/MLProject-Gantt-Chart.xlsx
+++ b/MLProject-Gantt-Chart.xlsx
@@ -29,6 +29,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">W</t>
     </r>
@@ -38,6 +39,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ing Yan Sang
 </t>
@@ -49,6 +51,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">I</t>
     </r>
@@ -58,19 +61,10 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">man Singh
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lim </t>
+Lim </t>
     </r>
     <r>
       <rPr>
@@ -178,7 +172,7 @@
     <numFmt numFmtId="169" formatCode="0%"/>
     <numFmt numFmtId="170" formatCode="M/D/YY"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -200,19 +194,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -351,11 +332,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,31 +345,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,7 +373,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -408,7 +381,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,11 +425,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,7 +465,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Calculation" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -510,14 +483,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFAFD3C5"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF5B9BD5"/>
-      <rgbColor rgb="FFC14B3A"/>
+      <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFBBE6EF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFB86FD7"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -532,10 +505,10 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF72C9DE"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFD5A8E7"/>
-      <rgbColor rgb="FFE3B3AA"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -545,7 +518,7 @@
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF528E77"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -557,7 +530,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1473,11 +1446,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="24303725"/>
-        <c:axId val="68834283"/>
+        <c:axId val="50636433"/>
+        <c:axId val="13795969"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="24303725"/>
+        <c:axId val="50636433"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1513,14 +1486,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68834283"/>
+        <c:crossAx val="13795969"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68834283"/>
+        <c:axId val="13795969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43051"/>
@@ -1568,7 +1541,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24303725"/>
+        <c:crossAx val="50636433"/>
         <c:crossesAt val="1"/>
         <c:majorUnit val="5"/>
       </c:valAx>
@@ -1607,9 +1580,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>1041120</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>317160</xdr:rowOff>
+      <xdr:rowOff>316800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1618,7 +1591,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9503280" y="2844360"/>
-        <a:ext cx="9414360" cy="7785000"/>
+        <a:ext cx="9411120" cy="7784640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1637,9 +1610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1653,7 +1626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="206280" y="12600"/>
-          <a:ext cx="18897480" cy="1485360"/>
+          <a:ext cx="18894600" cy="1485000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1674,9 +1647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>888480</xdr:colOff>
+      <xdr:colOff>888120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>870840</xdr:rowOff>
+      <xdr:rowOff>870480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1689,8 +1662,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15481800" y="588960"/>
-          <a:ext cx="3283200" cy="662760"/>
+          <a:off x="15480000" y="588960"/>
+          <a:ext cx="3281760" cy="662400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16920</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>313200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>48240</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>283320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="223200" y="7768080"/>
+          <a:ext cx="6132960" cy="2827440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1712,8 +1722,8 @@
   </sheetPr>
   <dimension ref="B1:V40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1723,16 +1733,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="12.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="10.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1755,767 +1765,764 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="7" t="n">
+      <c r="K4" s="5" t="n">
         <f aca="false">C5</f>
         <v>43036</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="9" t="n">
         <f aca="false">IF(ISBLANK(E5),"",E5+C5)</f>
         <v>43039</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="11" t="n">
         <f aca="false">IF(((D5)=""),"",(H5)*(D5-C5))</f>
         <v>0.15</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="11" t="n">
         <f aca="false">IF(F5="","",(D5-C5)-F5)</f>
         <v>2.85</v>
       </c>
-      <c r="H5" s="14" t="n">
+      <c r="H5" s="12" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="9" t="n">
         <f aca="false">IF(ISBLANK(E6),"",E6+C6)</f>
         <v>43040</v>
       </c>
-      <c r="E6" s="15" t="n">
+      <c r="E6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="11" t="n">
         <f aca="false">IF(((D6)=""),"",(H6)*(D6-C6))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="11" t="n">
         <f aca="false">IF(F6="","",(D6-C6)-F6)</f>
         <v>4</v>
       </c>
-      <c r="H6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16"/>
+      <c r="H6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="9" t="n">
         <f aca="false">IF(ISBLANK(E7),"",E7+C7)</f>
         <v>43040</v>
       </c>
-      <c r="E7" s="15" t="n">
+      <c r="E7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="11" t="n">
         <f aca="false">IF(((D7)=""),"",(H7)*(D7-C7))</f>
         <v>0</v>
       </c>
-      <c r="G7" s="13" t="n">
+      <c r="G7" s="11" t="n">
         <f aca="false">IF(F7="","",(D7-C7)-F7)</f>
         <v>4</v>
       </c>
-      <c r="H7" s="14" t="n">
+      <c r="H7" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="8" t="n">
         <v>43040</v>
       </c>
-      <c r="D8" s="11" t="n">
+      <c r="D8" s="9" t="n">
         <f aca="false">IF(ISBLANK(E8),"",E8+C8)</f>
         <v>43046</v>
       </c>
-      <c r="E8" s="15" t="n">
+      <c r="E8" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="11" t="n">
         <f aca="false">IF(((D8)=""),"",(H8)*(D8-C8))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="11" t="n">
         <f aca="false">IF(F8="","",(D8-C8)-F8)</f>
         <v>6</v>
       </c>
-      <c r="H8" s="14" t="n">
+      <c r="H8" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="8" t="n">
         <v>43043</v>
       </c>
-      <c r="D9" s="11" t="n">
+      <c r="D9" s="9" t="n">
         <f aca="false">IF(ISBLANK(E9),"",E9+C9)</f>
         <v>43049</v>
       </c>
-      <c r="E9" s="15" t="n">
+      <c r="E9" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="F9" s="13" t="n">
+      <c r="F9" s="11" t="n">
         <f aca="false">IF(((D9)=""),"",(H9)*(D9-C9))</f>
         <v>0</v>
       </c>
-      <c r="G9" s="13" t="n">
+      <c r="G9" s="11" t="n">
         <f aca="false">IF(F9="","",(D9-C9)-F9)</f>
         <v>6</v>
       </c>
-      <c r="H9" s="14" t="n">
+      <c r="H9" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="8" t="n">
         <v>43046</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="9" t="n">
         <f aca="false">IF(ISBLANK(E10),"",E10+C10)</f>
         <v>43051</v>
       </c>
-      <c r="E10" s="15" t="n">
+      <c r="E10" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="11" t="n">
         <f aca="false">IF(((D10)=""),"",(H10)*(D10-C10))</f>
         <v>0</v>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="11" t="n">
         <f aca="false">IF(F10="","",(D10-C10)-F10)</f>
         <v>5</v>
       </c>
-      <c r="H10" s="14" t="n">
+      <c r="H10" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D11" s="9" t="n">
         <f aca="false">IF(ISBLANK(E11),"",E11+C11)</f>
         <v>43036</v>
       </c>
-      <c r="E11" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13" t="n">
+      <c r="E11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11" t="n">
         <f aca="false">IF(((D11)=""),"",(H11)*(D11-C11))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G11" s="11" t="n">
         <f aca="false">IF(F11="","",(D11-C11)-F11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="14" t="n">
+      <c r="H11" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D12" s="11" t="n">
+      <c r="D12" s="9" t="n">
         <f aca="false">IF(ISBLANK(E12),"",E12+C12)</f>
         <v>43036</v>
       </c>
-      <c r="E12" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="13" t="n">
+      <c r="E12" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11" t="n">
         <f aca="false">IF(((D12)=""),"",(H12)*(D12-C12))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="13" t="n">
+      <c r="G12" s="11" t="n">
         <f aca="false">IF(F12="","",(D12-C12)-F12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="14" t="n">
+      <c r="H12" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="9" t="n">
         <f aca="false">IF(ISBLANK(E13),"",E13+C13)</f>
         <v>43036</v>
       </c>
-      <c r="E13" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13" t="n">
+      <c r="E13" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11" t="n">
         <f aca="false">IF(((D13)=""),"",(H13)*(D13-C13))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="13" t="n">
+      <c r="G13" s="11" t="n">
         <f aca="false">IF(F13="","",(D13-C13)-F13)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="14" t="n">
+      <c r="H13" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D14" s="11" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">IF(ISBLANK(E14),"",E14+C14)</f>
         <v>43036</v>
       </c>
-      <c r="E14" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="13" t="n">
+      <c r="E14" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11" t="n">
         <f aca="false">IF(((D14)=""),"",(H14)*(D14-C14))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="13" t="n">
+      <c r="G14" s="11" t="n">
         <f aca="false">IF(F14="","",(D14-C14)-F14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="14" t="n">
+      <c r="H14" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">IF(ISBLANK(E15),"",E15+C15)</f>
         <v>43036</v>
       </c>
-      <c r="E15" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="13" t="n">
+      <c r="E15" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11" t="n">
         <f aca="false">IF(((D15)=""),"",(H15)*(D15-C15))</f>
         <v>0</v>
       </c>
-      <c r="G15" s="13" t="n">
+      <c r="G15" s="11" t="n">
         <f aca="false">IF(F15="","",(D15-C15)-F15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="14" t="n">
+      <c r="H15" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D16" s="11" t="n">
+      <c r="D16" s="9" t="n">
         <f aca="false">IF(ISBLANK(E16),"",E16+C16)</f>
         <v>43036</v>
       </c>
-      <c r="E16" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="13" t="n">
+      <c r="E16" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11" t="n">
         <f aca="false">IF(((D16)=""),"",(H16)*(D16-C16))</f>
         <v>0</v>
       </c>
-      <c r="G16" s="13" t="n">
+      <c r="G16" s="11" t="n">
         <f aca="false">IF(F16="","",(D16-C16)-F16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="17"/>
+      <c r="H16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D17" s="9" t="n">
         <f aca="false">IF(ISBLANK(E17),"",E17+C17)</f>
         <v>43036</v>
       </c>
-      <c r="E17" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="13" t="n">
+      <c r="E17" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11" t="n">
         <f aca="false">IF(((D17)=""),"",(H17)*(D17-C17))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="11" t="n">
         <f aca="false">IF(F17="","",(D17-C17)-F17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="14" t="n">
+      <c r="H17" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D18" s="11" t="n">
+      <c r="D18" s="9" t="n">
         <f aca="false">IF(ISBLANK(E18),"",E18+C18)</f>
         <v>43036</v>
       </c>
-      <c r="E18" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="13" t="n">
+      <c r="E18" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11" t="n">
         <f aca="false">IF(((D18)=""),"",(H18)*(D18-C18))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="13" t="n">
+      <c r="G18" s="11" t="n">
         <f aca="false">IF(F18="","",(D18-C18)-F18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="14" t="n">
+      <c r="H18" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D19" s="11" t="n">
+      <c r="D19" s="9" t="n">
         <f aca="false">IF(ISBLANK(E19),"",E19+C19)</f>
         <v>43036</v>
       </c>
-      <c r="E19" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="13" t="n">
+      <c r="E19" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11" t="n">
         <f aca="false">IF(((D19)=""),"",(H19)*(D19-C19))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="13" t="n">
+      <c r="G19" s="11" t="n">
         <f aca="false">IF(F19="","",(D19-C19)-F19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="14" t="n">
+      <c r="H19" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="8" t="n">
         <v>43036</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="D20" s="9" t="n">
         <f aca="false">IF(ISBLANK(E20),"",E20+C20)</f>
         <v>43036</v>
       </c>
-      <c r="E20" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="13" t="n">
+      <c r="E20" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11" t="n">
         <f aca="false">IF(((D20)=""),"",(H20)*(D20-C20))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="13" t="n">
+      <c r="G20" s="11" t="n">
         <f aca="false">IF(F20="","",(D20-C20)-F20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="14" t="n">
+      <c r="H20" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="21"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="22"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11" t="str">
+      <c r="B22" s="20"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="str">
         <f aca="false">IF(ISBLANK(E22),"",E22+C22)</f>
         <v/>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="13" t="str">
+      <c r="E22" s="13"/>
+      <c r="F22" s="11" t="str">
         <f aca="false">IF(((D22)=""),"",(H22)*(D22-C22))</f>
         <v/>
       </c>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="11" t="str">
         <f aca="false">IF(F22="","",(D22-C22)-F22)</f>
         <v/>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11" t="str">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="str">
         <f aca="false">IF(ISBLANK(E23),"",E23+C23)</f>
         <v/>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="13" t="str">
+      <c r="E23" s="13"/>
+      <c r="F23" s="11" t="str">
         <f aca="false">IF(((D23)=""),"",(H23)*(D23-C23))</f>
         <v/>
       </c>
-      <c r="G23" s="13" t="str">
+      <c r="G23" s="11" t="str">
         <f aca="false">IF(F23="","",(D23-C23)-F23)</f>
         <v/>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11" t="str">
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9" t="str">
         <f aca="false">IF(ISBLANK(E24),"",E24+C24)</f>
         <v/>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="13" t="str">
+      <c r="E24" s="13"/>
+      <c r="F24" s="11" t="str">
         <f aca="false">IF(((D24)=""),"",(H24)*(D24-C24))</f>
         <v/>
       </c>
-      <c r="G24" s="13" t="str">
+      <c r="G24" s="11" t="str">
         <f aca="false">IF(F24="","",(D24-C24)-F24)</f>
         <v/>
       </c>
-      <c r="H24" s="14"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11" t="str">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="str">
         <f aca="false">IF(ISBLANK(E25),"",E25+C25)</f>
         <v/>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="13" t="str">
+      <c r="E25" s="13"/>
+      <c r="F25" s="11" t="str">
         <f aca="false">IF(((D25)=""),"",(H25)*(D25-C25))</f>
         <v/>
       </c>
-      <c r="G25" s="13" t="str">
+      <c r="G25" s="11" t="str">
         <f aca="false">IF(F25="","",(D25-C25)-F25)</f>
         <v/>
       </c>
-      <c r="H25" s="14"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11" t="str">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9" t="str">
         <f aca="false">IF(ISBLANK(E26),"",E26+C26)</f>
         <v/>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="13" t="str">
+      <c r="E26" s="13"/>
+      <c r="F26" s="11" t="str">
         <f aca="false">IF(((D26)=""),"",(H26)*(D26-C26))</f>
         <v/>
       </c>
-      <c r="G26" s="13" t="str">
+      <c r="G26" s="11" t="str">
         <f aca="false">IF(F26="","",(D26-C26)-F26)</f>
         <v/>
       </c>
-      <c r="H26" s="14"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11" t="str">
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9" t="str">
         <f aca="false">IF(ISBLANK(E27),"",E27+C27)</f>
         <v/>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="13" t="str">
+      <c r="E27" s="13"/>
+      <c r="F27" s="11" t="str">
         <f aca="false">IF(((D27)=""),"",(H27)*(D27-C27))</f>
         <v/>
       </c>
-      <c r="G27" s="13" t="str">
+      <c r="G27" s="11" t="str">
         <f aca="false">IF(F27="","",(D27-C27)-F27)</f>
         <v/>
       </c>
-      <c r="H27" s="14"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11" t="str">
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9" t="str">
         <f aca="false">IF(ISBLANK(E28),"",E28+C28)</f>
         <v/>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="13" t="str">
+      <c r="E28" s="13"/>
+      <c r="F28" s="11" t="str">
         <f aca="false">IF(((D28)=""),"",(H28)*(D28-C28))</f>
         <v/>
       </c>
-      <c r="G28" s="13" t="str">
+      <c r="G28" s="11" t="str">
         <f aca="false">IF(F28="","",(D28-C28)-F28)</f>
         <v/>
       </c>
-      <c r="H28" s="14"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11" t="str">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9" t="str">
         <f aca="false">IF(ISBLANK(E29),"",E29+C29)</f>
         <v/>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="13" t="str">
+      <c r="E29" s="13"/>
+      <c r="F29" s="11" t="str">
         <f aca="false">IF(((D29)=""),"",(H29)*(D29-C29))</f>
         <v/>
       </c>
-      <c r="G29" s="13" t="str">
+      <c r="G29" s="11" t="str">
         <f aca="false">IF(F29="","",(D29-C29)-F29)</f>
         <v/>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="23"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="16"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="23"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="16"/>
-      <c r="J31" s="24" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="14"/>
+      <c r="J31" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="25" t="s">
+      <c r="K31" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="26" t="s">
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="23"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="K32" s="27" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="K32" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27" t="s">
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
     </row>
     <row r="33" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="29"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="29"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="29"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="29"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="29"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>